<commit_message>
My wish test: adding new wish, and adding multiple wish lists
</commit_message>
<xml_diff>
--- a/data/Test_Plan_Projekat.xlsx
+++ b/data/Test_Plan_Projekat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LOGIN and LOG OUT" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="MyAddressTest" sheetId="3" r:id="rId3"/>
     <sheet name="BUG_MyAddressTest" sheetId="4" r:id="rId4"/>
     <sheet name="My_Personal_Info" sheetId="5" r:id="rId5"/>
+    <sheet name="My_Wishlist" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="118">
   <si>
     <t xml:space="preserve">Test steps: </t>
   </si>
@@ -541,12 +542,54 @@
   <si>
     <t>TC6:  Verify if it is possible to change personal information form for "MY PERSONAL INFORMATION" page</t>
   </si>
+  <si>
+    <t>Your personal information has been successfully updated.</t>
+  </si>
+  <si>
+    <t>The presonal informatio was successfully changed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> navigate to: http://automationpractice.com/</t>
+  </si>
+  <si>
+    <t>TC7:  Verify adding new WishList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on button "MY WISHLIST" </t>
+  </si>
+  <si>
+    <t>In input field "Name" enter name of wishlist</t>
+  </si>
+  <si>
+    <t>lista1</t>
+  </si>
+  <si>
+    <t>Click on green button "Save"</t>
+  </si>
+  <si>
+    <t>TC8:  Verify adding multiple WishLists</t>
+  </si>
+  <si>
+    <t>lista2</t>
+  </si>
+  <si>
+    <t>lista3</t>
+  </si>
+  <si>
+    <t>lista4</t>
+  </si>
+  <si>
+    <t>lista5</t>
+  </si>
+  <si>
+    <t>List with name: "lista2", "lista3",, "lista4", "lista5" were created and appeared in "MY WISHLIST" page</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,7 +675,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -885,11 +928,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1014,6 +1109,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1472,7 +1594,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.109375" customWidth="1"/>
@@ -1485,7 +1607,7 @@
     <col min="9" max="9" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1496,7 +1618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
@@ -1504,24 +1626,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="15" thickBot="1"/>
+    <row r="8" spans="1:9" ht="18">
       <c r="A8" s="24" t="s">
         <v>0</v>
       </c>
@@ -1546,7 +1668,7 @@
       </c>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="28.8">
       <c r="A9" s="19">
         <v>1</v>
       </c>
@@ -1561,7 +1683,7 @@
       <c r="H9" s="20"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" s="19">
         <v>2</v>
       </c>
@@ -1584,7 +1706,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="21">
         <v>3</v>
       </c>
@@ -1607,7 +1729,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" s="21">
         <v>4</v>
       </c>
@@ -1622,7 +1744,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="29.4" thickBot="1">
       <c r="A13" s="22" t="s">
         <v>39</v>
       </c>
@@ -1647,7 +1769,7 @@
       </c>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1656,7 +1778,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" s="14"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1666,7 +1788,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="43.2">
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
@@ -1690,7 +1812,7 @@
       </c>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="43.2">
       <c r="A17" s="8" t="s">
         <v>23</v>
       </c>
@@ -1714,7 +1836,7 @@
       </c>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9">
       <c r="A18" s="8"/>
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
@@ -1724,25 +1846,25 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9">
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="2"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="1:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" ht="18.600000000000001" thickBot="1">
       <c r="A21" s="30"/>
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="18">
       <c r="A22" s="24" t="s">
         <v>0</v>
       </c>
@@ -1754,7 +1876,7 @@
       <c r="E22" s="4"/>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="28.8">
       <c r="A23" s="19">
         <v>1</v>
       </c>
@@ -1766,7 +1888,7 @@
       <c r="E23" s="7"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9">
       <c r="A24" s="19">
         <v>2</v>
       </c>
@@ -1780,7 +1902,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9">
       <c r="A25" s="21">
         <v>3</v>
       </c>
@@ -1793,7 +1915,7 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9">
       <c r="A26" s="21">
         <v>4</v>
       </c>
@@ -1804,7 +1926,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="28.8">
       <c r="A27" s="21">
         <v>5</v>
       </c>
@@ -1813,7 +1935,7 @@
       </c>
       <c r="C27" s="28"/>
     </row>
-    <row r="28" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="29.4" thickBot="1">
       <c r="A28" s="22" t="s">
         <v>39</v>
       </c>
@@ -1822,7 +1944,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9">
       <c r="A31" s="8" t="s">
         <v>17</v>
       </c>
@@ -1830,7 +1952,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9">
       <c r="A32" s="8" t="s">
         <v>23</v>
       </c>
@@ -1852,9 +1974,9 @@
       <selection activeCell="J23" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="31" t="s">
         <v>54</v>
       </c>
@@ -1862,22 +1984,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" s="31"/>
       <c r="B6" s="31" t="s">
         <v>33</v>
@@ -1887,7 +2009,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="B7" s="5" t="s">
         <v>46</v>
       </c>
@@ -1895,7 +2017,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="B8" t="s">
         <v>47</v>
       </c>
@@ -1903,7 +2025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="B9" t="s">
         <v>48</v>
       </c>
@@ -1911,22 +2033,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="B10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" s="32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" s="32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" s="31" t="s">
         <v>54</v>
       </c>
@@ -1934,22 +2056,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" s="31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" s="32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" s="32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="31"/>
       <c r="B21" s="31" t="s">
         <v>33</v>
@@ -1958,7 +2080,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="B22" s="5" t="s">
         <v>46</v>
       </c>
@@ -1966,7 +2088,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="B23" t="s">
         <v>47</v>
       </c>
@@ -1974,7 +2096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="B24" t="s">
         <v>48</v>
       </c>
@@ -1982,17 +2104,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="B25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27" s="32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" s="32" t="s">
         <v>42</v>
       </c>
@@ -2010,14 +2132,14 @@
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="36.88671875" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2028,7 +2150,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
@@ -2036,24 +2158,24 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="15" thickBot="1"/>
+    <row r="8" spans="1:3" ht="18.600000000000001" thickBot="1">
       <c r="A8" s="44" t="s">
         <v>0</v>
       </c>
@@ -2062,7 +2184,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="28.8">
       <c r="A9" s="41">
         <v>1</v>
       </c>
@@ -2071,7 +2193,7 @@
       </c>
       <c r="C9" s="43"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="19">
         <v>2</v>
       </c>
@@ -2080,7 +2202,7 @@
       </c>
       <c r="C10" s="38"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="19">
         <v>3</v>
       </c>
@@ -2091,7 +2213,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="28.8">
       <c r="A12" s="19">
         <v>4</v>
       </c>
@@ -2100,7 +2222,7 @@
       </c>
       <c r="C12" s="39"/>
     </row>
-    <row r="13" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="29.4" thickBot="1">
       <c r="A13" s="22" t="s">
         <v>39</v>
       </c>
@@ -2109,7 +2231,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>64</v>
       </c>
@@ -2117,7 +2239,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>65</v>
       </c>
@@ -2125,12 +2247,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="47"/>
       <c r="B17" s="48"/>
       <c r="C17" s="49"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -2141,7 +2263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
         <v>55</v>
       </c>
@@ -2149,13 +2271,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="15" thickBot="1"/>
+    <row r="23" spans="1:3" ht="18.600000000000001" thickBot="1">
       <c r="A23" s="44" t="s">
         <v>0</v>
       </c>
@@ -2164,7 +2286,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="28.8">
       <c r="A24" s="41">
         <v>1</v>
       </c>
@@ -2173,7 +2295,7 @@
       </c>
       <c r="C24" s="43"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" s="19">
         <v>2</v>
       </c>
@@ -2182,7 +2304,7 @@
       </c>
       <c r="C25" s="38"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" s="19">
         <v>3</v>
       </c>
@@ -2193,7 +2315,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" s="41">
         <v>4</v>
       </c>
@@ -2204,7 +2326,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" s="19">
         <v>5</v>
       </c>
@@ -2215,7 +2337,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" s="19">
         <v>6</v>
       </c>
@@ -2226,7 +2348,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" s="41">
         <v>7</v>
       </c>
@@ -2237,7 +2359,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" s="19">
         <v>8</v>
       </c>
@@ -2248,7 +2370,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" s="19">
         <v>9</v>
       </c>
@@ -2259,7 +2381,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3">
       <c r="A33" s="41">
         <v>10</v>
       </c>
@@ -2270,7 +2392,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3">
       <c r="A34" s="41">
         <v>11</v>
       </c>
@@ -2279,7 +2401,7 @@
       </c>
       <c r="C34" s="39"/>
     </row>
-    <row r="35" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="29.4" thickBot="1">
       <c r="A35" s="22" t="s">
         <v>39</v>
       </c>
@@ -2288,7 +2410,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
         <v>64</v>
       </c>
@@ -2296,7 +2418,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
         <v>65</v>
       </c>
@@ -2304,12 +2426,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3">
       <c r="A39" s="47"/>
       <c r="B39" s="48"/>
       <c r="C39" s="49"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
         <v>3</v>
       </c>
@@ -2320,7 +2442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
@@ -2328,13 +2450,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" ht="15" thickBot="1"/>
+    <row r="45" spans="1:3" ht="18.600000000000001" thickBot="1">
       <c r="A45" s="44" t="s">
         <v>0</v>
       </c>
@@ -2343,7 +2465,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3">
       <c r="A46" s="41">
         <v>1</v>
       </c>
@@ -2352,7 +2474,7 @@
       </c>
       <c r="C46" s="43"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3">
       <c r="A47" s="19">
         <v>2</v>
       </c>
@@ -2361,7 +2483,7 @@
       </c>
       <c r="C47" s="38"/>
     </row>
-    <row r="48" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" ht="29.4" thickBot="1">
       <c r="A48" s="22" t="s">
         <v>39</v>
       </c>
@@ -2370,7 +2492,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>17</v>
       </c>
@@ -2378,7 +2500,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>65</v>
       </c>
@@ -2403,9 +2525,9 @@
       <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" s="31" t="s">
         <v>54</v>
       </c>
@@ -2413,25 +2535,25 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" s="31" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" s="31"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" s="32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" s="32" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" s="31"/>
       <c r="B7" s="31" t="s">
         <v>33</v>
@@ -2441,7 +2563,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
@@ -2449,7 +2571,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="B9" t="s">
         <v>47</v>
       </c>
@@ -2457,7 +2579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="B10" t="s">
         <v>48</v>
       </c>
@@ -2465,22 +2587,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="B11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="B12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="B13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="B14" t="s">
         <v>72</v>
       </c>
@@ -2488,22 +2610,22 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="B15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1">
       <c r="A17" s="32" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1">
       <c r="A19" s="32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
         <v>77</v>
       </c>
@@ -2517,20 +2639,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
     <col min="2" max="2" width="36.88671875" customWidth="1"/>
     <col min="3" max="3" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2541,7 +2663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
@@ -2550,30 +2672,30 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>103</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="15" thickBot="1">
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="18.600000000000001" thickBot="1">
       <c r="A8" s="44" t="s">
         <v>0</v>
       </c>
@@ -2582,7 +2704,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="28.8">
       <c r="A9" s="41">
         <v>1</v>
       </c>
@@ -2591,7 +2713,7 @@
       </c>
       <c r="C9" s="43"/>
     </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="28.8">
       <c r="A10" s="19">
         <v>2</v>
       </c>
@@ -2602,7 +2724,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="28.8">
       <c r="A11" s="19">
         <v>3</v>
       </c>
@@ -2613,7 +2735,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="28.8">
       <c r="A12" s="19"/>
       <c r="B12" s="50" t="s">
         <v>102</v>
@@ -2622,7 +2744,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="19">
         <v>4</v>
       </c>
@@ -2631,7 +2753,7 @@
       </c>
       <c r="C13" s="39"/>
     </row>
-    <row r="14" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="29.4" thickBot="1">
       <c r="A14" s="22" t="s">
         <v>39</v>
       </c>
@@ -2640,7 +2762,288 @@
         <v>36</v>
       </c>
     </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="6" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="53"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" thickBot="1">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="18.600000000000001" thickBot="1">
+      <c r="A8" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="45"/>
+      <c r="C8" s="46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="41">
+        <v>1</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="43"/>
+    </row>
+    <row r="10" spans="1:3" ht="28.8">
+      <c r="A10" s="19">
+        <v>2</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="19">
+        <v>3</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="38"/>
+    </row>
+    <row r="12" spans="1:3" ht="29.4" thickBot="1">
+      <c r="A12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="53"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="18.600000000000001" thickBot="1">
+      <c r="A25" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="45"/>
+      <c r="C25" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="41">
+        <v>1</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="54"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+    </row>
+    <row r="27" spans="1:6" ht="28.8">
+      <c r="A27" s="19">
+        <v>2</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="19">
+        <v>3</v>
+      </c>
+      <c r="B28" s="50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="55"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+    </row>
+    <row r="29" spans="1:6" ht="29.4" thickBot="1">
+      <c r="A29" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="23"/>
+      <c r="C29" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B18:C18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
multiple adding wishlists successfully pass
</commit_message>
<xml_diff>
--- a/data/Test_Plan_Projekat.xlsx
+++ b/data/Test_Plan_Projekat.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="121">
   <si>
     <t xml:space="preserve">Test steps: </t>
   </si>
@@ -583,6 +583,15 @@
   </si>
   <si>
     <t>List with name: "lista2", "lista3",, "lista4", "lista5" were created and appeared in "MY WISHLIST" page</t>
+  </si>
+  <si>
+    <t>Click on  button "Delete" and delete one wish list</t>
+  </si>
+  <si>
+    <t>List with name: "lista2" was removed successfully from "MY WISHLISTS"</t>
+  </si>
+  <si>
+    <t>TC9:  Verify deleting one wish list</t>
   </si>
 </sst>
 </file>
@@ -643,7 +652,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -674,6 +683,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -984,7 +999,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1116,26 +1131,30 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2184,7 +2203,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="28.8">
+    <row r="9" spans="1:3">
       <c r="A9" s="41">
         <v>1</v>
       </c>
@@ -2213,7 +2232,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.8">
+    <row r="12" spans="1:3">
       <c r="A12" s="19">
         <v>4</v>
       </c>
@@ -2286,7 +2305,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.8">
+    <row r="24" spans="1:3">
       <c r="A24" s="41">
         <v>1</v>
       </c>
@@ -2786,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2804,10 +2823,10 @@
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="53"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
@@ -2903,146 +2922,249 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>106</v>
-      </c>
-      <c r="C18" s="53"/>
+    <row r="17" spans="1:6">
+      <c r="A17" s="60"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="59"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-    </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="1"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="1"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickBot="1">
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:6" ht="18.600000000000001" thickBot="1">
-      <c r="A25" s="44" t="s">
+    <row r="25" spans="1:6" ht="15" thickBot="1">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" ht="18.600000000000001" thickBot="1">
+      <c r="A26" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="45"/>
-      <c r="C25" s="46" t="s">
+      <c r="B26" s="45"/>
+      <c r="C26" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="59" t="s">
+      <c r="D26" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="46" t="s">
+      <c r="E26" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="46" t="s">
+      <c r="F26" s="46" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="41">
+    <row r="27" spans="1:6">
+      <c r="A27" s="41">
         <v>1</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B27" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-    </row>
-    <row r="27" spans="1:6" ht="28.8">
-      <c r="A27" s="19">
+      <c r="C27" s="53"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+    </row>
+    <row r="28" spans="1:6" ht="28.8">
+      <c r="A28" s="19">
         <v>2</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B28" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C28" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="57" t="s">
+      <c r="D28" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E28" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="F27" s="38" t="s">
+      <c r="F28" s="38" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="19">
+    <row r="29" spans="1:6">
+      <c r="A29" s="19">
         <v>3</v>
       </c>
-      <c r="B28" s="50" t="s">
+      <c r="B29" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="55"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-    </row>
-    <row r="29" spans="1:6" ht="29.4" thickBot="1">
-      <c r="A29" s="22" t="s">
+      <c r="C29" s="54"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+    </row>
+    <row r="30" spans="1:6" ht="29.4" thickBot="1">
+      <c r="A30" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="56" t="s">
+      <c r="B30" s="23"/>
+      <c r="C30" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D30" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="40" t="s">
+      <c r="E30" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F30" s="40" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="51" t="s">
+    <row r="32" spans="1:6">
+      <c r="A32" s="51" t="s">
         <v>17</v>
-      </c>
-      <c r="B31" s="52" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="B32" s="52" t="s">
         <v>117</v>
       </c>
     </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" s="59"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1"/>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" ht="15" thickBot="1">
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" ht="18.600000000000001" thickBot="1">
+      <c r="A43" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="45"/>
+      <c r="C43" s="46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="41">
+        <v>1</v>
+      </c>
+      <c r="B44" s="42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="43"/>
+    </row>
+    <row r="45" spans="1:3" ht="28.8">
+      <c r="A45" s="19">
+        <v>3</v>
+      </c>
+      <c r="B45" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="61" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="29.4" thickBot="1">
+      <c r="A46" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48" s="52" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="52" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>